<commit_message>
Advancing the scripts for the evaluation section
</commit_message>
<xml_diff>
--- a/evaluation/results/improvements-formatting.xlsx
+++ b/evaluation/results/improvements-formatting.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9EEDA44-26AD-46D6-9660-FCEA52BF2BEB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bruto" sheetId="1" r:id="rId1"/>
     <sheet name="Paper" sheetId="2" r:id="rId2"/>
     <sheet name="Paper 2" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -176,11 +177,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -250,20 +251,26 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>504266</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>571501</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>112058</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>419526</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>134470</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>486762</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>56029</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1025" name="Picture 1"/>
+        <xdr:cNvPr id="1025" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -277,7 +284,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="12091148" y="4190999"/>
+          <a:off x="12393707" y="4684058"/>
           <a:ext cx="7781790" cy="3753971"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -308,7 +315,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2049" name="Picture 1"/>
+        <xdr:cNvPr id="2049" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000001080000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -353,7 +366,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3073" name="Picture 1"/>
+        <xdr:cNvPr id="3073" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000010C0000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -393,7 +412,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagem 2"/>
+        <xdr:cNvPr id="3" name="Imagem 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -674,27 +699,25 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O42"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="10" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -726,7 +749,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -757,12 +780,12 @@
       <c r="J2" s="1">
         <v>16.2762304463945</v>
       </c>
-      <c r="O2" s="2" t="str">
-        <f>A2 &amp; " &amp; " &amp; TEXT(B2,"0.0")&amp;" &amp; "&amp;TEXT(E2,"0.0")&amp;" $\pm$ "&amp;TEXT(F2,"0.0")&amp;" &amp; "&amp;TEXT(C2,"0.0")&amp;" &amp; "&amp;TEXT(I2,"0.0")&amp;" &amp; "&amp;TEXT(G2,"0.0")&amp;" $\pm$ "&amp;TEXT(H2,"0.0")&amp;" &amp; "&amp;TEXT(D2,"0.0")&amp;" &amp; "&amp;TEXT(J2,"0.0")&amp;" \\"</f>
+      <c r="M2" s="2" t="str">
+        <f t="shared" ref="M2:M20" si="0">A2 &amp; " &amp; " &amp; TEXT(B2,"0.0")&amp;" &amp; "&amp;TEXT(E2,"0.0")&amp;" $\pm$ "&amp;TEXT(F2,"0.0")&amp;" &amp; "&amp;TEXT(C2,"0.0")&amp;" &amp; "&amp;TEXT(I2,"0.0")&amp;" &amp; "&amp;TEXT(G2,"0.0")&amp;" $\pm$ "&amp;TEXT(H2,"0.0")&amp;" &amp; "&amp;TEXT(D2,"0.0")&amp;" &amp; "&amp;TEXT(J2,"0.0")&amp;" \\"</f>
         <v>browserify &amp; 25.4 &amp; 25.2 $\pm$ 0.3 &amp; 25.4 &amp; 25.4 &amp; 13.5 $\pm$ 2.9 &amp; 14.2 &amp; 16.3 \\</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -793,12 +816,12 @@
       <c r="J3" s="1">
         <v>24.208009563658099</v>
       </c>
-      <c r="O3" s="2" t="str">
-        <f>A3 &amp; " &amp; " &amp; TEXT(B3,"0.0")&amp;" &amp; "&amp;TEXT(E3,"0.0")&amp;" $\pm$ "&amp;TEXT(F3,"0.0")&amp;" &amp; "&amp;TEXT(C3,"0.0")&amp;" &amp; "&amp;TEXT(I3,"0.0")&amp;" &amp; "&amp;TEXT(G3,"0.0")&amp;" $\pm$ "&amp;TEXT(H3,"0.0")&amp;" &amp; "&amp;TEXT(D3,"0.0")&amp;" &amp; "&amp;TEXT(J3,"0.0")&amp;" \\"</f>
+      <c r="M3" s="2" t="str">
+        <f t="shared" si="0"/>
         <v>d3-node &amp; 26.0 &amp; 26.0 $\pm$ 0.0 &amp; 26.0 &amp; 26.0 &amp; 24.2 $\pm$ 0.0 &amp; 24.2 &amp; 24.2 \\</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -829,12 +852,12 @@
       <c r="J4" s="1">
         <v>9.2216367214779993</v>
       </c>
-      <c r="O4" s="2" t="str">
-        <f>A4 &amp; " &amp; " &amp; TEXT(B4,"0.0")&amp;" &amp; "&amp;TEXT(E4,"0.0")&amp;" $\pm$ "&amp;TEXT(F4,"0.0")&amp;" &amp; "&amp;TEXT(C4,"0.0")&amp;" &amp; "&amp;TEXT(I4,"0.0")&amp;" &amp; "&amp;TEXT(G4,"0.0")&amp;" $\pm$ "&amp;TEXT(H4,"0.0")&amp;" &amp; "&amp;TEXT(D4,"0.0")&amp;" &amp; "&amp;TEXT(J4,"0.0")&amp;" \\"</f>
+      <c r="M4" s="2" t="str">
+        <f t="shared" si="0"/>
         <v>decimal.js &amp; 15.0 &amp; 6.4 $\pm$ 2.0 &amp; 7.0 &amp; 9.2 &amp; 6.4 $\pm$ 2.0 &amp; 7.0 &amp; 9.2 \\</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -865,12 +888,12 @@
       <c r="J5" s="1">
         <v>0.63942367024558699</v>
       </c>
-      <c r="O5" s="2" t="str">
-        <f>A5 &amp; " &amp; " &amp; TEXT(B5,"0.0")&amp;" &amp; "&amp;TEXT(E5,"0.0")&amp;" $\pm$ "&amp;TEXT(F5,"0.0")&amp;" &amp; "&amp;TEXT(C5,"0.0")&amp;" &amp; "&amp;TEXT(I5,"0.0")&amp;" &amp; "&amp;TEXT(G5,"0.0")&amp;" $\pm$ "&amp;TEXT(H5,"0.0")&amp;" &amp; "&amp;TEXT(D5,"0.0")&amp;" &amp; "&amp;TEXT(J5,"0.0")&amp;" \\"</f>
+      <c r="M5" s="2" t="str">
+        <f t="shared" si="0"/>
         <v>esprima &amp; 3.9 &amp; 3.9 $\pm$ 0.0 &amp; 3.9 &amp; 3.9 &amp; 0.3 $\pm$ 0.1 &amp; 0.3 &amp; 0.6 \\</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -901,12 +924,12 @@
       <c r="J6" s="1">
         <v>23.589468027942001</v>
       </c>
-      <c r="O6" s="2" t="str">
-        <f>A6 &amp; " &amp; " &amp; TEXT(B6,"0.0")&amp;" &amp; "&amp;TEXT(E6,"0.0")&amp;" $\pm$ "&amp;TEXT(F6,"0.0")&amp;" &amp; "&amp;TEXT(C6,"0.0")&amp;" &amp; "&amp;TEXT(I6,"0.0")&amp;" &amp; "&amp;TEXT(G6,"0.0")&amp;" $\pm$ "&amp;TEXT(H6,"0.0")&amp;" &amp; "&amp;TEXT(D6,"0.0")&amp;" &amp; "&amp;TEXT(J6,"0.0")&amp;" \\"</f>
+      <c r="M6" s="2" t="str">
+        <f t="shared" si="0"/>
         <v>exectimer &amp; 26.8 &amp; 26.4 $\pm$ 0.5 &amp; 26.8 &amp; 26.8 &amp; 22.8 $\pm$ 0.8 &amp; 23.1 &amp; 23.6 \\</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -937,12 +960,12 @@
       <c r="J7" s="1">
         <v>11.2432803385566</v>
       </c>
-      <c r="O7" s="2" t="str">
-        <f>A7 &amp; " &amp; " &amp; TEXT(B7,"0.0")&amp;" &amp; "&amp;TEXT(E7,"0.0")&amp;" $\pm$ "&amp;TEXT(F7,"0.0")&amp;" &amp; "&amp;TEXT(C7,"0.0")&amp;" &amp; "&amp;TEXT(I7,"0.0")&amp;" &amp; "&amp;TEXT(G7,"0.0")&amp;" $\pm$ "&amp;TEXT(H7,"0.0")&amp;" &amp; "&amp;TEXT(D7,"0.0")&amp;" &amp; "&amp;TEXT(J7,"0.0")&amp;" \\"</f>
+      <c r="M7" s="2" t="str">
+        <f t="shared" si="0"/>
         <v>express &amp; 15.9 &amp; 15.7 $\pm$ 0.3 &amp; 15.9 &amp; 15.9 &amp; 8.6 $\pm$ 1.3 &amp; 8.3 &amp; 11.2 \\</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -973,12 +996,12 @@
       <c r="J8" s="1">
         <v>27.7687052924535</v>
       </c>
-      <c r="O8" s="2" t="str">
-        <f>A8 &amp; " &amp; " &amp; TEXT(B8,"0.0")&amp;" &amp; "&amp;TEXT(E8,"0.0")&amp;" $\pm$ "&amp;TEXT(F8,"0.0")&amp;" &amp; "&amp;TEXT(C8,"0.0")&amp;" &amp; "&amp;TEXT(I8,"0.0")&amp;" &amp; "&amp;TEXT(G8,"0.0")&amp;" $\pm$ "&amp;TEXT(H8,"0.0")&amp;" &amp; "&amp;TEXT(D8,"0.0")&amp;" &amp; "&amp;TEXT(J8,"0.0")&amp;" \\"</f>
+      <c r="M8" s="2" t="str">
+        <f t="shared" si="0"/>
         <v>jquery &amp; 80.1 &amp; 80.1 $\pm$ 0.0 &amp; 80.1 &amp; 80.1 &amp; 20.8 $\pm$ 3.8 &amp; 20.0 &amp; 27.8 \\</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1009,12 +1032,12 @@
       <c r="J9" s="1">
         <v>1.5553227496172199</v>
       </c>
-      <c r="O9" s="2" t="str">
-        <f>A9 &amp; " &amp; " &amp; TEXT(B9,"0.0")&amp;" &amp; "&amp;TEXT(E9,"0.0")&amp;" $\pm$ "&amp;TEXT(F9,"0.0")&amp;" &amp; "&amp;TEXT(C9,"0.0")&amp;" &amp; "&amp;TEXT(I9,"0.0")&amp;" &amp; "&amp;TEXT(G9,"0.0")&amp;" $\pm$ "&amp;TEXT(H9,"0.0")&amp;" &amp; "&amp;TEXT(D9,"0.0")&amp;" &amp; "&amp;TEXT(J9,"0.0")&amp;" \\"</f>
+      <c r="M9" s="2" t="str">
+        <f t="shared" si="0"/>
         <v>lodash &amp; 1.6 &amp; 1.2 $\pm$ 0.3 &amp; 1.2 &amp; 1.5 &amp; 1.2 $\pm$ 0.3 &amp; 1.3 &amp; 1.6 \\</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -1045,12 +1068,12 @@
       <c r="J10" s="1">
         <v>21.004937869661902</v>
       </c>
-      <c r="O10" s="2" t="str">
-        <f>A10 &amp; " &amp; " &amp; TEXT(B10,"0.0")&amp;" &amp; "&amp;TEXT(E10,"0.0")&amp;" $\pm$ "&amp;TEXT(F10,"0.0")&amp;" &amp; "&amp;TEXT(C10,"0.0")&amp;" &amp; "&amp;TEXT(I10,"0.0")&amp;" &amp; "&amp;TEXT(G10,"0.0")&amp;" $\pm$ "&amp;TEXT(H10,"0.0")&amp;" &amp; "&amp;TEXT(D10,"0.0")&amp;" &amp; "&amp;TEXT(J10,"0.0")&amp;" \\"</f>
+      <c r="M10" s="2" t="str">
+        <f t="shared" si="0"/>
         <v>mathjs &amp; 27.0 &amp; 19.1 $\pm$ 1.3 &amp; 19.0 &amp; 21.0 &amp; 19.1 $\pm$ 1.3 &amp; 19.0 &amp; 21.0 \\</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -1081,12 +1104,12 @@
       <c r="J11" s="1">
         <v>1.95809000343524</v>
       </c>
-      <c r="O11" s="2" t="str">
-        <f>A11 &amp; " &amp; " &amp; TEXT(B11,"0.0")&amp;" &amp; "&amp;TEXT(E11,"0.0")&amp;" $\pm$ "&amp;TEXT(F11,"0.0")&amp;" &amp; "&amp;TEXT(C11,"0.0")&amp;" &amp; "&amp;TEXT(I11,"0.0")&amp;" &amp; "&amp;TEXT(G11,"0.0")&amp;" $\pm$ "&amp;TEXT(H11,"0.0")&amp;" &amp; "&amp;TEXT(D11,"0.0")&amp;" &amp; "&amp;TEXT(J11,"0.0")&amp;" \\"</f>
+      <c r="M11" s="2" t="str">
+        <f t="shared" si="0"/>
         <v>minimist &amp; 2.8 &amp; 2.8 $\pm$ 0.0 &amp; 2.8 &amp; 2.8 &amp; 1.9 $\pm$ 0.1 &amp; 1.8 &amp; 2.0 \\</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -1117,12 +1140,12 @@
       <c r="J12" s="1">
         <v>2.3215660169332901</v>
       </c>
-      <c r="O12" s="2" t="str">
-        <f>A12 &amp; " &amp; " &amp; TEXT(B12,"0.0")&amp;" &amp; "&amp;TEXT(E12,"0.0")&amp;" $\pm$ "&amp;TEXT(F12,"0.0")&amp;" &amp; "&amp;TEXT(C12,"0.0")&amp;" &amp; "&amp;TEXT(I12,"0.0")&amp;" &amp; "&amp;TEXT(G12,"0.0")&amp;" $\pm$ "&amp;TEXT(H12,"0.0")&amp;" &amp; "&amp;TEXT(D12,"0.0")&amp;" &amp; "&amp;TEXT(J12,"0.0")&amp;" \\"</f>
+      <c r="M12" s="2" t="str">
+        <f t="shared" si="0"/>
         <v>moment &amp; 7.2 &amp; 7.1 $\pm$ 0.4 &amp; 7.2 &amp; 7.2 &amp; 1.6 $\pm$ 0.3 &amp; 1.4 &amp; 2.3 \\</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -1153,12 +1176,12 @@
       <c r="J13" s="1">
         <v>5.6104349724390197</v>
       </c>
-      <c r="O13" s="2" t="str">
-        <f>A13 &amp; " &amp; " &amp; TEXT(B13,"0.0")&amp;" &amp; "&amp;TEXT(E13,"0.0")&amp;" $\pm$ "&amp;TEXT(F13,"0.0")&amp;" &amp; "&amp;TEXT(C13,"0.0")&amp;" &amp; "&amp;TEXT(I13,"0.0")&amp;" &amp; "&amp;TEXT(G13,"0.0")&amp;" $\pm$ "&amp;TEXT(H13,"0.0")&amp;" &amp; "&amp;TEXT(D13,"0.0")&amp;" &amp; "&amp;TEXT(J13,"0.0")&amp;" \\"</f>
+      <c r="M13" s="2" t="str">
+        <f t="shared" si="0"/>
         <v>node-semver &amp; 13.5 &amp; 13.4 $\pm$ 0.3 &amp; 13.4 &amp; 13.7 &amp; 4.4 $\pm$ 0.7 &amp; 4.1 &amp; 5.6 \\</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -1189,12 +1212,12 @@
       <c r="J14" s="1">
         <v>61.270125223613597</v>
       </c>
-      <c r="O14" s="2" t="str">
-        <f>A14 &amp; " &amp; " &amp; TEXT(B14,"0.0")&amp;" &amp; "&amp;TEXT(E14,"0.0")&amp;" $\pm$ "&amp;TEXT(F14,"0.0")&amp;" &amp; "&amp;TEXT(C14,"0.0")&amp;" &amp; "&amp;TEXT(I14,"0.0")&amp;" &amp; "&amp;TEXT(G14,"0.0")&amp;" $\pm$ "&amp;TEXT(H14,"0.0")&amp;" &amp; "&amp;TEXT(D14,"0.0")&amp;" &amp; "&amp;TEXT(J14,"0.0")&amp;" \\"</f>
+      <c r="M14" s="2" t="str">
+        <f t="shared" si="0"/>
         <v>plivo-node &amp; 15.3 &amp; 15.9 $\pm$ 0.4 &amp; 15.9 &amp; 16.4 &amp; 56.1 $\pm$ 3.0 &amp; 55.6 &amp; 61.3 \\</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1225,12 +1248,12 @@
       <c r="J15" s="1">
         <v>33.854818523153902</v>
       </c>
-      <c r="O15" s="2" t="str">
-        <f>A15 &amp; " &amp; " &amp; TEXT(B15,"0.0")&amp;" &amp; "&amp;TEXT(E15,"0.0")&amp;" $\pm$ "&amp;TEXT(F15,"0.0")&amp;" &amp; "&amp;TEXT(C15,"0.0")&amp;" &amp; "&amp;TEXT(I15,"0.0")&amp;" &amp; "&amp;TEXT(G15,"0.0")&amp;" $\pm$ "&amp;TEXT(H15,"0.0")&amp;" &amp; "&amp;TEXT(D15,"0.0")&amp;" &amp; "&amp;TEXT(J15,"0.0")&amp;" \\"</f>
+      <c r="M15" s="2" t="str">
+        <f t="shared" si="0"/>
         <v>pug &amp; 39.4 &amp; 39.4 $\pm$ 0.0 &amp; 39.4 &amp; 39.4 &amp; 30.6 $\pm$ 2.2 &amp; 31.1 &amp; 33.9 \\</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -1261,12 +1284,12 @@
       <c r="J16" s="1">
         <v>64.053426248548206</v>
       </c>
-      <c r="O16" s="2" t="str">
-        <f>A16 &amp; " &amp; " &amp; TEXT(B16,"0.0")&amp;" &amp; "&amp;TEXT(E16,"0.0")&amp;" $\pm$ "&amp;TEXT(F16,"0.0")&amp;" &amp; "&amp;TEXT(C16,"0.0")&amp;" &amp; "&amp;TEXT(I16,"0.0")&amp;" &amp; "&amp;TEXT(G16,"0.0")&amp;" $\pm$ "&amp;TEXT(H16,"0.0")&amp;" &amp; "&amp;TEXT(D16,"0.0")&amp;" &amp; "&amp;TEXT(J16,"0.0")&amp;" \\"</f>
+      <c r="M16" s="2" t="str">
+        <f t="shared" si="0"/>
         <v>tleaf &amp; 65.8 &amp; 65.8 $\pm$ 0.0 &amp; 65.8 &amp; 65.8 &amp; 63.7 $\pm$ 0.8 &amp; 64.0 &amp; 64.1 \\</v>
       </c>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1297,12 +1320,12 @@
       <c r="J17" s="1">
         <v>4.0785372370032302</v>
       </c>
-      <c r="O17" s="2" t="str">
-        <f>A17 &amp; " &amp; " &amp; TEXT(B17,"0.0")&amp;" &amp; "&amp;TEXT(E17,"0.0")&amp;" $\pm$ "&amp;TEXT(F17,"0.0")&amp;" &amp; "&amp;TEXT(C17,"0.0")&amp;" &amp; "&amp;TEXT(I17,"0.0")&amp;" &amp; "&amp;TEXT(G17,"0.0")&amp;" $\pm$ "&amp;TEXT(H17,"0.0")&amp;" &amp; "&amp;TEXT(D17,"0.0")&amp;" &amp; "&amp;TEXT(J17,"0.0")&amp;" \\"</f>
+      <c r="M17" s="2" t="str">
+        <f t="shared" si="0"/>
         <v>UglifyJS2 &amp; 13.2 &amp; 12.2 $\pm$ 4.1 &amp; 13.9 &amp; 13.9 &amp; 3.1 $\pm$ 0.6 &amp; 3.1 &amp; 4.1 \\</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -1333,12 +1356,12 @@
       <c r="J18" s="1">
         <v>8.0237741456166507</v>
       </c>
-      <c r="O18" s="2" t="str">
-        <f>A18 &amp; " &amp; " &amp; TEXT(B18,"0.0")&amp;" &amp; "&amp;TEXT(E18,"0.0")&amp;" $\pm$ "&amp;TEXT(F18,"0.0")&amp;" &amp; "&amp;TEXT(C18,"0.0")&amp;" &amp; "&amp;TEXT(I18,"0.0")&amp;" &amp; "&amp;TEXT(G18,"0.0")&amp;" $\pm$ "&amp;TEXT(H18,"0.0")&amp;" &amp; "&amp;TEXT(D18,"0.0")&amp;" &amp; "&amp;TEXT(J18,"0.0")&amp;" \\"</f>
+      <c r="M18" s="2" t="str">
+        <f t="shared" si="0"/>
         <v>underscore &amp; 11.5 &amp; 11.5 $\pm$ 0.0 &amp; 11.5 &amp; 11.5 &amp; 4.6 $\pm$ 1.5 &amp; 4.7 &amp; 8.0 \\</v>
       </c>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -1369,12 +1392,12 @@
       <c r="J19" s="1">
         <v>24.3484735666419</v>
       </c>
-      <c r="O19" s="2" t="str">
-        <f>A19 &amp; " &amp; " &amp; TEXT(B19,"0.0")&amp;" &amp; "&amp;TEXT(E19,"0.0")&amp;" $\pm$ "&amp;TEXT(F19,"0.0")&amp;" &amp; "&amp;TEXT(C19,"0.0")&amp;" &amp; "&amp;TEXT(I19,"0.0")&amp;" &amp; "&amp;TEXT(G19,"0.0")&amp;" $\pm$ "&amp;TEXT(H19,"0.0")&amp;" &amp; "&amp;TEXT(D19,"0.0")&amp;" &amp; "&amp;TEXT(J19,"0.0")&amp;" \\"</f>
+      <c r="M19" s="2" t="str">
+        <f t="shared" si="0"/>
         <v>uuid &amp; 20.8 &amp; 21.4 $\pm$ 2.5 &amp; 22.2 &amp; 23.6 &amp; 21.5 $\pm$ 1.9 &amp; 21.6 &amp; 24.3 \\</v>
       </c>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -1405,648 +1428,648 @@
       <c r="J20" s="1">
         <v>17.608537472714001</v>
       </c>
-      <c r="O20" s="2" t="str">
-        <f>A20 &amp; " &amp; " &amp; TEXT(B20,"0.0")&amp;" &amp; "&amp;TEXT(E20,"0.0")&amp;" $\pm$ "&amp;TEXT(F20,"0.0")&amp;" &amp; "&amp;TEXT(C20,"0.0")&amp;" &amp; "&amp;TEXT(I20,"0.0")&amp;" &amp; "&amp;TEXT(G20,"0.0")&amp;" $\pm$ "&amp;TEXT(H20,"0.0")&amp;" &amp; "&amp;TEXT(D20,"0.0")&amp;" &amp; "&amp;TEXT(J20,"0.0")&amp;" \\"</f>
+      <c r="M20" s="2" t="str">
+        <f t="shared" si="0"/>
         <v>xml2js &amp; 4.1 &amp; -2.2 $\pm$ 4.4 &amp; -1.2 &amp; 2.8 &amp; 10.3 $\pm$ 5.8 &amp; 9.8 &amp; 17.6 \\</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
-      <c r="A23" s="3" t="s">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B25" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C25" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D25" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="E25" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F25" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G23" s="3" t="s">
+      <c r="G25" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H23" s="3" t="s">
+      <c r="H25" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I23" s="3" t="s">
+      <c r="I25" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J23" s="3" t="s">
+      <c r="J25" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:15">
-      <c r="A24" t="s">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B26" s="1">
         <v>26.6</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C26" s="1">
         <v>1.6</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D26" s="1">
         <v>13.2</v>
       </c>
-      <c r="E24" s="1">
+      <c r="E26" s="1">
         <v>1.7</v>
       </c>
-      <c r="F24" s="1">
+      <c r="F26" s="1">
         <v>0</v>
       </c>
-      <c r="G24" s="1">
+      <c r="G26" s="1">
         <v>12.8</v>
       </c>
-      <c r="H24" s="1">
+      <c r="H26" s="1">
         <v>2.9</v>
       </c>
-      <c r="I24" s="1">
+      <c r="I26" s="1">
         <v>1.7</v>
       </c>
-      <c r="J24" s="1">
+      <c r="J26" s="1">
         <v>16.3</v>
       </c>
     </row>
-    <row r="25" spans="1:15">
-      <c r="A25" t="s">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>29</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B27" s="1">
         <v>29.3</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C27" s="1">
         <v>29.3</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D27" s="1">
         <v>25.5</v>
       </c>
-      <c r="E25" s="1">
+      <c r="E27" s="1">
         <v>29.3</v>
       </c>
-      <c r="F25" s="1">
+      <c r="F27" s="1">
         <v>0</v>
       </c>
-      <c r="G25" s="1">
+      <c r="G27" s="1">
         <v>25.5</v>
       </c>
-      <c r="H25" s="1">
+      <c r="H27" s="1">
         <v>0</v>
       </c>
-      <c r="I25" s="1">
+      <c r="I27" s="1">
         <v>29.3</v>
       </c>
-      <c r="J25" s="1">
+      <c r="J27" s="1">
         <v>25.5</v>
       </c>
     </row>
-    <row r="26" spans="1:15">
-      <c r="A26" t="s">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>46</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B28" s="1">
         <v>7.1</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C28" s="1">
         <v>7.2</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D28" s="1">
         <v>4.8</v>
       </c>
-      <c r="E26" s="1">
+      <c r="E28" s="1">
         <v>8.8000000000000007</v>
       </c>
-      <c r="F26" s="1">
+      <c r="F28" s="1">
         <v>4.4000000000000004</v>
       </c>
-      <c r="G26" s="1">
+      <c r="G28" s="1">
         <v>4.4000000000000004</v>
       </c>
-      <c r="H26" s="1">
+      <c r="H28" s="1">
         <v>1.8</v>
       </c>
-      <c r="I26" s="1">
+      <c r="I28" s="1">
         <v>18.100000000000001</v>
       </c>
-      <c r="J26" s="1">
+      <c r="J28" s="1">
         <v>6.8</v>
       </c>
     </row>
-    <row r="27" spans="1:15">
-      <c r="A27" t="s">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B29" s="1">
         <v>4</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C29" s="1">
         <v>4.9000000000000004</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D29" s="1">
         <v>0.3</v>
       </c>
-      <c r="E27" s="1">
+      <c r="E29" s="1">
         <v>4.8</v>
       </c>
-      <c r="F27" s="1">
+      <c r="F29" s="1">
         <v>0.2</v>
       </c>
-      <c r="G27" s="1">
+      <c r="G29" s="1">
         <v>0.4</v>
       </c>
-      <c r="H27" s="1">
+      <c r="H29" s="1">
         <v>0.1</v>
       </c>
-      <c r="I27" s="1">
+      <c r="I29" s="1">
         <v>4.9000000000000004</v>
       </c>
-      <c r="J27" s="1">
+      <c r="J29" s="1">
         <v>0.6</v>
       </c>
     </row>
-    <row r="28" spans="1:15">
-      <c r="A28" t="s">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B30" s="1">
         <v>22.8</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C30" s="1">
         <v>22.8</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D30" s="1">
         <v>20.8</v>
       </c>
-      <c r="E28" s="1">
+      <c r="E30" s="1">
         <v>22.8</v>
       </c>
-      <c r="F28" s="1">
+      <c r="F30" s="1">
         <v>0</v>
       </c>
-      <c r="G28" s="1">
+      <c r="G30" s="1">
         <v>20.7</v>
       </c>
-      <c r="H28" s="1">
+      <c r="H30" s="1">
         <v>0.8</v>
       </c>
-      <c r="I28" s="1">
+      <c r="I30" s="1">
         <v>22.8</v>
       </c>
-      <c r="J28" s="1">
+      <c r="J30" s="1">
         <v>21.4</v>
       </c>
     </row>
-    <row r="29" spans="1:15">
-      <c r="A29" t="s">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>32</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B31" s="1">
         <v>3.4</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C31" s="1">
         <v>8</v>
       </c>
-      <c r="D29" s="1">
+      <c r="D31" s="1">
         <v>4.3</v>
       </c>
-      <c r="E29" s="1">
+      <c r="E31" s="1">
         <v>7.6</v>
       </c>
-      <c r="F29" s="1">
+      <c r="F31" s="1">
         <v>1.5</v>
       </c>
-      <c r="G29" s="1">
+      <c r="G31" s="1">
         <v>4.4000000000000004</v>
       </c>
-      <c r="H29" s="1">
+      <c r="H31" s="1">
         <v>0.7</v>
       </c>
-      <c r="I29" s="1">
+      <c r="I31" s="1">
         <v>8.4</v>
       </c>
-      <c r="J29" s="1">
+      <c r="J31" s="1">
         <v>5.7</v>
       </c>
     </row>
-    <row r="30" spans="1:15">
-      <c r="A30" t="s">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>33</v>
       </c>
-      <c r="B30" s="1">
+      <c r="B32" s="1">
         <v>58.3</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C32" s="1">
         <v>58.4</v>
       </c>
-      <c r="D30" s="1">
+      <c r="D32" s="1">
         <v>17.3</v>
       </c>
-      <c r="E30" s="1">
+      <c r="E32" s="1">
         <v>58.9</v>
       </c>
-      <c r="F30" s="1">
+      <c r="F32" s="1">
         <v>1.5</v>
       </c>
-      <c r="G30" s="1">
+      <c r="G32" s="1">
         <v>17.8</v>
       </c>
-      <c r="H30" s="1">
+      <c r="H32" s="1">
         <v>3.3</v>
       </c>
-      <c r="I30" s="1">
+      <c r="I32" s="1">
         <v>62.5</v>
       </c>
-      <c r="J30" s="1">
+      <c r="J32" s="1">
         <v>25.4</v>
       </c>
     </row>
-    <row r="31" spans="1:15">
-      <c r="A31" t="s">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>34</v>
       </c>
-      <c r="B31" s="1">
+      <c r="B33" s="1">
         <v>2.7</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C33" s="1">
         <v>5.9</v>
       </c>
-      <c r="D31" s="1">
+      <c r="D33" s="1">
         <v>0.6</v>
       </c>
-      <c r="E31" s="1">
+      <c r="E33" s="1">
         <v>5.5</v>
       </c>
-      <c r="F31" s="1">
+      <c r="F33" s="1">
         <v>0.9</v>
       </c>
-      <c r="G31" s="1">
+      <c r="G33" s="1">
         <v>0.6</v>
-      </c>
-      <c r="H31" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="I31" s="1">
-        <v>6</v>
-      </c>
-      <c r="J31" s="1">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15">
-      <c r="A32" t="s">
-        <v>35</v>
-      </c>
-      <c r="B32" s="1">
-        <v>9.8000000000000007</v>
-      </c>
-      <c r="C32" s="1">
-        <v>27.8</v>
-      </c>
-      <c r="D32" s="1">
-        <v>15.8</v>
-      </c>
-      <c r="E32" s="1">
-        <v>22.1</v>
-      </c>
-      <c r="F32" s="1">
-        <v>9.8000000000000007</v>
-      </c>
-      <c r="G32" s="1">
-        <v>15.8</v>
-      </c>
-      <c r="H32" s="1">
-        <v>0.9</v>
-      </c>
-      <c r="I32" s="1">
-        <v>30.4</v>
-      </c>
-      <c r="J32" s="1">
-        <v>17.2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10">
-      <c r="A33" t="s">
-        <v>36</v>
-      </c>
-      <c r="B33" s="1">
-        <v>2.8</v>
-      </c>
-      <c r="C33" s="1">
-        <v>2.8</v>
-      </c>
-      <c r="D33" s="1">
-        <v>1.8</v>
-      </c>
-      <c r="E33" s="1">
-        <v>2.7</v>
-      </c>
-      <c r="F33" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="G33" s="1">
-        <v>1.8</v>
       </c>
       <c r="H33" s="1">
         <v>0.1</v>
       </c>
       <c r="I33" s="1">
+        <v>6</v>
+      </c>
+      <c r="J33" s="1">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" s="1">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="C34" s="1">
+        <v>27.8</v>
+      </c>
+      <c r="D34" s="1">
+        <v>15.8</v>
+      </c>
+      <c r="E34" s="1">
+        <v>22.1</v>
+      </c>
+      <c r="F34" s="1">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="G34" s="1">
+        <v>15.8</v>
+      </c>
+      <c r="H34" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="I34" s="1">
+        <v>30.4</v>
+      </c>
+      <c r="J34" s="1">
+        <v>17.2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" s="1">
         <v>2.8</v>
       </c>
-      <c r="J33" s="1">
+      <c r="C35" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="D35" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="E35" s="1">
+        <v>2.7</v>
+      </c>
+      <c r="F35" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="G35" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="H35" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="I35" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="J35" s="1">
         <v>1.9</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
-      <c r="A34" t="s">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>37</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B36" s="1">
         <v>7.1</v>
       </c>
-      <c r="C34" s="1">
+      <c r="C36" s="1">
         <v>5.5</v>
       </c>
-      <c r="D34" s="1">
+      <c r="D36" s="1">
         <v>1.4</v>
       </c>
-      <c r="E34" s="1">
+      <c r="E36" s="1">
         <v>5.5</v>
       </c>
-      <c r="F34" s="1">
+      <c r="F36" s="1">
         <v>0</v>
       </c>
-      <c r="G34" s="1">
+      <c r="G36" s="1">
         <v>1.5</v>
       </c>
-      <c r="H34" s="1">
+      <c r="H36" s="1">
         <v>0.2</v>
       </c>
-      <c r="I34" s="1">
+      <c r="I36" s="1">
         <v>5.5</v>
       </c>
-      <c r="J34" s="1">
+      <c r="J36" s="1">
         <v>1.9</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
-      <c r="A35" t="s">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>38</v>
       </c>
-      <c r="B35" s="1">
+      <c r="B37" s="1">
         <v>0.2</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C37" s="1">
         <v>3</v>
       </c>
-      <c r="D35" s="1">
+      <c r="D37" s="1">
         <v>4.0999999999999996</v>
       </c>
-      <c r="E35" s="1">
+      <c r="E37" s="1">
         <v>3.2</v>
       </c>
-      <c r="F35" s="1">
+      <c r="F37" s="1">
         <v>1.9</v>
       </c>
-      <c r="G35" s="1">
+      <c r="G37" s="1">
         <v>4.0999999999999996</v>
       </c>
-      <c r="H35" s="1">
+      <c r="H37" s="1">
         <v>0.46</v>
       </c>
-      <c r="I35" s="1">
+      <c r="I37" s="1">
         <v>6.8</v>
       </c>
-      <c r="J35" s="1">
+      <c r="J37" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
-      <c r="A36" t="s">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>39</v>
       </c>
-      <c r="B36" s="1">
+      <c r="B38" s="1">
         <v>33.200000000000003</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C38" s="1">
         <v>15.6</v>
       </c>
-      <c r="D36" s="1">
+      <c r="D38" s="1">
         <v>55.5</v>
       </c>
-      <c r="E36" s="1">
+      <c r="E38" s="1">
         <v>16.7</v>
       </c>
-      <c r="F36" s="1">
+      <c r="F38" s="1">
         <v>5</v>
       </c>
-      <c r="G36" s="1">
+      <c r="G38" s="1">
         <v>55.2</v>
       </c>
-      <c r="H36" s="1">
+      <c r="H38" s="1">
         <v>2.5</v>
       </c>
-      <c r="I36" s="1">
+      <c r="I38" s="1">
         <v>23.4</v>
       </c>
-      <c r="J36" s="1">
+      <c r="J38" s="1">
         <v>58.5</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
-      <c r="A37" t="s">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>40</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B39" s="1">
         <v>30.9</v>
       </c>
-      <c r="C37" s="1">
+      <c r="C39" s="1">
         <v>31.4</v>
       </c>
-      <c r="D37" s="1">
+      <c r="D39" s="1">
         <v>23.9</v>
       </c>
-      <c r="E37" s="1">
+      <c r="E39" s="1">
         <v>31.4</v>
       </c>
-      <c r="F37" s="1">
+      <c r="F39" s="1">
         <v>0</v>
       </c>
-      <c r="G37" s="1">
+      <c r="G39" s="1">
         <v>23.3</v>
       </c>
-      <c r="H37" s="1">
+      <c r="H39" s="1">
         <v>1.7</v>
       </c>
-      <c r="I37" s="1">
+      <c r="I39" s="1">
         <v>31.4</v>
       </c>
-      <c r="J37" s="1">
+      <c r="J39" s="1">
         <v>26.1</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
-      <c r="A38" t="s">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>41</v>
       </c>
-      <c r="B38" s="1">
+      <c r="B40" s="1">
         <v>73.8</v>
       </c>
-      <c r="C38" s="1">
+      <c r="C40" s="1">
         <v>73.8</v>
       </c>
-      <c r="D38" s="1">
+      <c r="D40" s="1">
         <v>69.5</v>
       </c>
-      <c r="E38" s="1">
+      <c r="E40" s="1">
         <v>73.8</v>
-      </c>
-      <c r="F38" s="1">
-        <v>0</v>
-      </c>
-      <c r="G38" s="1">
-        <v>69.2</v>
-      </c>
-      <c r="H38" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="I38" s="1">
-        <v>73.8</v>
-      </c>
-      <c r="J38" s="1">
-        <v>69.599999999999994</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10">
-      <c r="A39" t="s">
-        <v>42</v>
-      </c>
-      <c r="B39" s="1">
-        <v>12.1</v>
-      </c>
-      <c r="C39" s="1">
-        <v>10.9</v>
-      </c>
-      <c r="D39" s="1">
-        <v>2.7</v>
-      </c>
-      <c r="E39" s="1">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="F39" s="1">
-        <v>3.9</v>
-      </c>
-      <c r="G39" s="1">
-        <v>2.7</v>
-      </c>
-      <c r="H39" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="I39" s="1">
-        <v>15.3</v>
-      </c>
-      <c r="J39" s="1">
-        <v>3.7</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10">
-      <c r="A40" t="s">
-        <v>43</v>
-      </c>
-      <c r="B40" s="1">
-        <v>10</v>
-      </c>
-      <c r="C40" s="1">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="D40" s="1">
-        <v>3.7</v>
-      </c>
-      <c r="E40" s="1">
-        <v>5.0999999999999996</v>
       </c>
       <c r="F40" s="1">
         <v>0</v>
       </c>
       <c r="G40" s="1">
+        <v>69.2</v>
+      </c>
+      <c r="H40" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="I40" s="1">
+        <v>73.8</v>
+      </c>
+      <c r="J40" s="1">
+        <v>69.599999999999994</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41" s="1">
+        <v>12.1</v>
+      </c>
+      <c r="C41" s="1">
+        <v>10.9</v>
+      </c>
+      <c r="D41" s="1">
+        <v>2.7</v>
+      </c>
+      <c r="E41" s="1">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="F41" s="1">
+        <v>3.9</v>
+      </c>
+      <c r="G41" s="1">
+        <v>2.7</v>
+      </c>
+      <c r="H41" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="I41" s="1">
+        <v>15.3</v>
+      </c>
+      <c r="J41" s="1">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>43</v>
+      </c>
+      <c r="B42" s="1">
+        <v>10</v>
+      </c>
+      <c r="C42" s="1">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="D42" s="1">
+        <v>3.7</v>
+      </c>
+      <c r="E42" s="1">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="F42" s="1">
+        <v>0</v>
+      </c>
+      <c r="G42" s="1">
         <v>3.8</v>
       </c>
-      <c r="H40" s="1">
+      <c r="H42" s="1">
         <v>1.2</v>
       </c>
-      <c r="I40" s="1">
+      <c r="I42" s="1">
         <v>5.0999999999999996</v>
       </c>
-      <c r="J40" s="1">
+      <c r="J42" s="1">
         <v>6.6</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
-      <c r="A41" t="s">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>44</v>
       </c>
-      <c r="B41" s="1">
+      <c r="B43" s="1">
         <v>24.3</v>
       </c>
-      <c r="C41" s="1">
+      <c r="C43" s="1">
         <v>23.3</v>
       </c>
-      <c r="D41" s="1">
+      <c r="D43" s="1">
         <v>23.2</v>
       </c>
-      <c r="E41" s="1">
+      <c r="E43" s="1">
         <v>22.3</v>
       </c>
-      <c r="F41" s="1">
+      <c r="F43" s="1">
         <v>3.3</v>
       </c>
-      <c r="G41" s="1">
+      <c r="G43" s="1">
         <v>23.4</v>
       </c>
-      <c r="H41" s="1">
+      <c r="H43" s="1">
         <v>2</v>
       </c>
-      <c r="I41" s="1">
+      <c r="I43" s="1">
         <v>24.7</v>
       </c>
-      <c r="J41" s="1">
+      <c r="J43" s="1">
         <v>26.4</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
-      <c r="A42" t="s">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>45</v>
       </c>
-      <c r="B42" s="1">
+      <c r="B44" s="1">
         <v>5</v>
       </c>
-      <c r="C42" s="1">
+      <c r="C44" s="1">
         <v>2</v>
       </c>
-      <c r="D42" s="1">
+      <c r="D44" s="1">
         <v>8.6</v>
       </c>
-      <c r="E42" s="1">
+      <c r="E44" s="1">
         <v>2.2999999999999998</v>
       </c>
-      <c r="F42" s="1">
+      <c r="F44" s="1">
         <v>0.9</v>
       </c>
-      <c r="G42" s="1">
+      <c r="G44" s="1">
         <v>9.1999999999999993</v>
       </c>
-      <c r="H42" s="1">
+      <c r="H44" s="1">
         <v>5</v>
       </c>
-      <c r="I42" s="1">
+      <c r="I44" s="1">
         <v>4.5999999999999996</v>
       </c>
-      <c r="J42" s="1">
+      <c r="J44" s="1">
         <v>15.2</v>
       </c>
     </row>
@@ -2058,27 +2081,37 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" scale="74" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:T42"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" scale="74" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update on formatting worksheet
</commit_message>
<xml_diff>
--- a/evaluation/results/improvements-formatting.xlsx
+++ b/evaluation/results/improvements-formatting.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9EEDA44-26AD-46D6-9660-FCEA52BF2BEB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84D70373-87F1-4ECD-AF5B-BF7F15DE4D1D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -225,11 +225,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -709,7 +710,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -753,31 +756,31 @@
       <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="4">
         <v>25.402518122853898</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="4">
         <v>25.402518122853898</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="4">
         <v>14.2006867607783</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="4">
         <v>25.2483784814956</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="4">
         <v>0.32495489627572699</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="4">
         <v>13.5017169019458</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2" s="4">
         <v>2.8645170726948899</v>
       </c>
-      <c r="I2" s="1">
+      <c r="I2" s="4">
         <v>25.402518122853898</v>
       </c>
-      <c r="J2" s="1">
+      <c r="J2" s="4">
         <v>16.2762304463945</v>
       </c>
       <c r="M2" s="2" t="str">
@@ -789,31 +792,31 @@
       <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="4">
         <v>26.001195457262401</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="4">
         <v>26.001195457262401</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="4">
         <v>24.208009563658099</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="4">
         <v>26.001195457262401</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="4">
         <v>0</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="4">
         <v>24.208009563658099</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="4">
         <v>0</v>
       </c>
-      <c r="I3" s="1">
+      <c r="I3" s="4">
         <v>26.001195457262401</v>
       </c>
-      <c r="J3" s="1">
+      <c r="J3" s="4">
         <v>24.208009563658099</v>
       </c>
       <c r="M3" s="2" t="str">
@@ -825,31 +828,31 @@
       <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="4">
         <v>14.980001269760599</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="4">
         <v>6.9836835756459896</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="4">
         <v>6.9836835756459896</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="4">
         <v>6.4386388165830697</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="4">
         <v>2.0484810750834899</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="4">
         <v>6.4386388165830697</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4" s="4">
         <v>2.0484810750834899</v>
       </c>
-      <c r="I4" s="1">
+      <c r="I4" s="4">
         <v>9.2216367214779993</v>
       </c>
-      <c r="J4" s="1">
+      <c r="J4" s="4">
         <v>9.2216367214779993</v>
       </c>
       <c r="M4" s="2" t="str">
@@ -861,31 +864,31 @@
       <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="4">
         <v>3.8751079846970198</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="4">
         <v>3.88204985807725</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="4">
         <v>0.33243860298655098</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="4">
         <v>3.88097001110699</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="4">
         <v>5.0277290557317802E-3</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="4">
         <v>0.34686227323213698</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H5" s="4">
         <v>0.113633505179756</v>
       </c>
-      <c r="I5" s="1">
+      <c r="I5" s="4">
         <v>3.8859064543996</v>
       </c>
-      <c r="J5" s="1">
+      <c r="J5" s="4">
         <v>0.63942367024558699</v>
       </c>
       <c r="M5" s="2" t="str">
@@ -897,31 +900,31 @@
       <c r="A6" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="4">
         <v>26.759806555615299</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="4">
         <v>26.759806555615299</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="4">
         <v>23.052122514777</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="4">
         <v>26.372917786136501</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="4">
         <v>0.49947125367532602</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="4">
         <v>22.847931219774299</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="4">
         <v>0.846515808002401</v>
       </c>
-      <c r="I6" s="1">
+      <c r="I6" s="4">
         <v>26.759806555615299</v>
       </c>
-      <c r="J6" s="1">
+      <c r="J6" s="4">
         <v>23.589468027942001</v>
       </c>
       <c r="M6" s="2" t="str">
@@ -933,31 +936,31 @@
       <c r="A7" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="4">
         <v>15.8869953105341</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="4">
         <v>15.864119867322399</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="4">
         <v>8.3152236074573906</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="4">
         <v>15.6982729040375</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="4">
         <v>0.30468405375112101</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="4">
         <v>8.5611346219832996</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7" s="4">
         <v>1.34721763199808</v>
       </c>
-      <c r="I7" s="1">
+      <c r="I7" s="4">
         <v>15.8869953105341</v>
       </c>
-      <c r="J7" s="1">
+      <c r="J7" s="4">
         <v>11.2432803385566</v>
       </c>
       <c r="M7" s="2" t="str">
@@ -969,31 +972,31 @@
       <c r="A8" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="4">
         <v>80.102122961565897</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="4">
         <v>80.0532465441498</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="4">
         <v>20.0163304735837</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="4">
         <v>80.054971594176195</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="4">
         <v>3.3594624437759797E-2</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="4">
         <v>20.789037882098601</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8" s="4">
         <v>3.8186520050014501</v>
       </c>
-      <c r="I8" s="1">
+      <c r="I8" s="4">
         <v>80.1251236285852</v>
       </c>
-      <c r="J8" s="1">
+      <c r="J8" s="4">
         <v>27.7687052924535</v>
       </c>
       <c r="M8" s="2" t="str">
@@ -1005,31 +1008,31 @@
       <c r="A9" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="4">
         <v>1.5895720847771799</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="4">
         <v>1.21585139817874</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="4">
         <v>1.2742767346280901</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="4">
         <v>1.2029575308244</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="4">
         <v>0.25567215903386598</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9" s="4">
         <v>1.2059795309855701</v>
       </c>
-      <c r="H9" s="1">
+      <c r="H9" s="4">
         <v>0.27776467990707399</v>
       </c>
-      <c r="I9" s="1">
+      <c r="I9" s="4">
         <v>1.4807800789749399</v>
       </c>
-      <c r="J9" s="1">
+      <c r="J9" s="4">
         <v>1.5553227496172199</v>
       </c>
       <c r="M9" s="2" t="str">
@@ -1041,31 +1044,31 @@
       <c r="A10" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="4">
         <v>27.036192956752899</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="4">
         <v>19.037929350480201</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="4">
         <v>19.037929350480201</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="4">
         <v>19.0729285365457</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="4">
         <v>1.27451902212885</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10" s="4">
         <v>19.0729285365457</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H10" s="4">
         <v>1.27451902212885</v>
       </c>
-      <c r="I10" s="1">
+      <c r="I10" s="4">
         <v>21.004937869661902</v>
       </c>
-      <c r="J10" s="1">
+      <c r="J10" s="4">
         <v>21.004937869661902</v>
       </c>
       <c r="M10" s="2" t="str">
@@ -1077,31 +1080,31 @@
       <c r="A11" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="4">
         <v>2.7825489522500901</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="4">
         <v>2.7825489522500901</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="4">
         <v>1.83785640673308</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="4">
         <v>2.7825489522500901</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="4">
         <v>0</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11" s="4">
         <v>1.8515973892133299</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H11" s="4">
         <v>8.3284537024930202E-2</v>
       </c>
-      <c r="I11" s="1">
+      <c r="I11" s="4">
         <v>2.7825489522500901</v>
       </c>
-      <c r="J11" s="1">
+      <c r="J11" s="4">
         <v>1.95809000343524</v>
       </c>
       <c r="M11" s="2" t="str">
@@ -1113,31 +1116,31 @@
       <c r="A12" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="4">
         <v>7.2291376627630903</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="4">
         <v>7.2291376627630903</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="4">
         <v>1.43121632585134</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="4">
         <v>7.1245188764228997</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="4">
         <v>0.35180866260960802</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G12" s="4">
         <v>1.5508310623868899</v>
       </c>
-      <c r="H12" s="1">
+      <c r="H12" s="4">
         <v>0.34101859580845401</v>
       </c>
-      <c r="I12" s="1">
+      <c r="I12" s="4">
         <v>7.2455163377282696</v>
       </c>
-      <c r="J12" s="1">
+      <c r="J12" s="4">
         <v>2.3215660169332901</v>
       </c>
       <c r="M12" s="2" t="str">
@@ -1149,31 +1152,31 @@
       <c r="A13" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="4">
         <v>13.4639524095399</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="4">
         <v>13.4011897615019</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="4">
         <v>4.11504666266441</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="4">
         <v>13.424657534246601</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13" s="4">
         <v>0.34178637998953998</v>
       </c>
-      <c r="G13" s="1">
+      <c r="G13" s="4">
         <v>4.3519074387382002</v>
       </c>
-      <c r="H13" s="1">
+      <c r="H13" s="4">
         <v>0.65127719015951202</v>
       </c>
-      <c r="I13" s="1">
+      <c r="I13" s="4">
         <v>13.7095453801233</v>
       </c>
-      <c r="J13" s="1">
+      <c r="J13" s="4">
         <v>5.6104349724390197</v>
       </c>
       <c r="M13" s="2" t="str">
@@ -1185,31 +1188,31 @@
       <c r="A14" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="4">
         <v>15.342799188640999</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="4">
         <v>15.9026369168357</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="4">
         <v>55.6228655065864</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="4">
         <v>15.922920892494901</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14" s="4">
         <v>0.38062357712973499</v>
       </c>
-      <c r="G14" s="1">
+      <c r="G14" s="4">
         <v>56.118881118881099</v>
       </c>
-      <c r="H14" s="1">
+      <c r="H14" s="4">
         <v>2.9594665942510798</v>
       </c>
-      <c r="I14" s="1">
+      <c r="I14" s="4">
         <v>16.381338742393499</v>
       </c>
-      <c r="J14" s="1">
+      <c r="J14" s="4">
         <v>61.270125223613597</v>
       </c>
       <c r="M14" s="2" t="str">
@@ -1221,31 +1224,31 @@
       <c r="A15" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="4">
         <v>39.3541666666667</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="4">
         <v>39.3541666666667</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15" s="4">
         <v>31.0909470171047</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15" s="4">
         <v>39.3541666666667</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F15" s="4">
         <v>0</v>
       </c>
-      <c r="G15" s="1">
+      <c r="G15" s="4">
         <v>30.607008760951199</v>
       </c>
-      <c r="H15" s="1">
+      <c r="H15" s="4">
         <v>2.1976540599659602</v>
       </c>
-      <c r="I15" s="1">
+      <c r="I15" s="4">
         <v>39.3541666666667</v>
       </c>
-      <c r="J15" s="1">
+      <c r="J15" s="4">
         <v>33.854818523153902</v>
       </c>
       <c r="M15" s="2" t="str">
@@ -1257,31 +1260,31 @@
       <c r="A16" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="4">
         <v>65.795586527293807</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="4">
         <v>65.795586527293807</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16" s="4">
         <v>64.024390243902403</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" s="4">
         <v>65.795586527293807</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F16" s="4">
         <v>0</v>
       </c>
-      <c r="G16" s="1">
+      <c r="G16" s="4">
         <v>63.710801393728197</v>
       </c>
-      <c r="H16" s="1">
+      <c r="H16" s="4">
         <v>0.81090837378076497</v>
       </c>
-      <c r="I16" s="1">
+      <c r="I16" s="4">
         <v>65.795586527293807</v>
       </c>
-      <c r="J16" s="1">
+      <c r="J16" s="4">
         <v>64.053426248548206</v>
       </c>
       <c r="M16" s="2" t="str">
@@ -1293,31 +1296,31 @@
       <c r="A17" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="4">
         <v>13.2041077591005</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="4">
         <v>13.881776689302001</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17" s="4">
         <v>3.1434376043637999</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E17" s="4">
         <v>12.2319937660025</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F17" s="4">
         <v>4.0677785065038199</v>
       </c>
-      <c r="G17" s="1">
+      <c r="G17" s="4">
         <v>3.0564677724590901</v>
       </c>
-      <c r="H17" s="1">
+      <c r="H17" s="4">
         <v>0.57501879421457602</v>
       </c>
-      <c r="I17" s="1">
+      <c r="I17" s="4">
         <v>13.9443949682734</v>
       </c>
-      <c r="J17" s="1">
+      <c r="J17" s="4">
         <v>4.0785372370032302</v>
       </c>
       <c r="M17" s="2" t="str">
@@ -1329,31 +1332,31 @@
       <c r="A18" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="4">
         <v>11.478250108285399</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="4">
         <v>11.481343976239099</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18" s="4">
         <v>4.6588657751362099</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E18" s="4">
         <v>11.481343976239099</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F18" s="4">
         <v>3.2612231711793001E-3</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G18" s="4">
         <v>4.6266716196136697</v>
       </c>
-      <c r="H18" s="1">
+      <c r="H18" s="4">
         <v>1.49206258268059</v>
       </c>
-      <c r="I18" s="1">
+      <c r="I18" s="4">
         <v>11.484437844192801</v>
       </c>
-      <c r="J18" s="1">
+      <c r="J18" s="4">
         <v>8.0237741456166507</v>
       </c>
       <c r="M18" s="2" t="str">
@@ -1365,31 +1368,31 @@
       <c r="A19" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="4">
         <v>20.824025812856799</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="4">
         <v>22.151898734177198</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D19" s="4">
         <v>21.568627450980401</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E19" s="4">
         <v>21.429635145197299</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F19" s="4">
         <v>2.4916445024892901</v>
       </c>
-      <c r="G19" s="1">
+      <c r="G19" s="4">
         <v>21.451973194341001</v>
       </c>
-      <c r="H19" s="1">
+      <c r="H19" s="4">
         <v>1.8572909493508301</v>
       </c>
-      <c r="I19" s="1">
+      <c r="I19" s="4">
         <v>23.628691983122401</v>
       </c>
-      <c r="J19" s="1">
+      <c r="J19" s="4">
         <v>24.3484735666419</v>
       </c>
       <c r="M19" s="2" t="str">
@@ -1401,31 +1404,31 @@
       <c r="A20" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="4">
         <v>4.1199855439103796</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" s="4">
         <v>-1.15046379954222</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20" s="4">
         <v>9.7501819063788506</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E20" s="4">
         <v>-2.1900975786049899</v>
       </c>
-      <c r="F20" s="1">
+      <c r="F20" s="4">
         <v>4.3954368272869697</v>
       </c>
-      <c r="G20" s="1">
+      <c r="G20" s="4">
         <v>10.325006063546001</v>
       </c>
-      <c r="H20" s="1">
+      <c r="H20" s="4">
         <v>5.7897045024873002</v>
       </c>
-      <c r="I20" s="1">
+      <c r="I20" s="4">
         <v>2.7948439946994399</v>
       </c>
-      <c r="J20" s="1">
+      <c r="J20" s="4">
         <v>17.608537472714001</v>
       </c>
       <c r="M20" s="2" t="str">

</xml_diff>

<commit_message>
Adjustment in evaluation scripts
</commit_message>
<xml_diff>
--- a/evaluation/results/improvements-formatting.xlsx
+++ b/evaluation/results/improvements-formatting.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84D70373-87F1-4ECD-AF5B-BF7F15DE4D1D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Bruto" sheetId="1" r:id="rId1"/>
     <sheet name="Paper" sheetId="2" r:id="rId2"/>
     <sheet name="Paper 2" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="31">
   <si>
     <t>instance</t>
   </si>
@@ -57,63 +56,9 @@
     <t>shc_max</t>
   </si>
   <si>
-    <t>browserify</t>
-  </si>
-  <si>
-    <t>d3-node</t>
-  </si>
-  <si>
-    <t>decimal.js</t>
-  </si>
-  <si>
-    <t>esprima</t>
-  </si>
-  <si>
-    <t>exectimer</t>
-  </si>
-  <si>
-    <t>express</t>
-  </si>
-  <si>
-    <t>jquery</t>
-  </si>
-  <si>
-    <t>lodash</t>
-  </si>
-  <si>
-    <t>mathjs</t>
-  </si>
-  <si>
-    <t>minimist</t>
-  </si>
-  <si>
-    <t>moment</t>
-  </si>
-  <si>
-    <t>node-semver</t>
-  </si>
-  <si>
-    <t>plivo-node</t>
-  </si>
-  <si>
-    <t>pug</t>
-  </si>
-  <si>
-    <t>tleaf</t>
-  </si>
-  <si>
     <t>UglifyJS2</t>
   </si>
   <si>
-    <t>underscore</t>
-  </si>
-  <si>
-    <t>uuid</t>
-  </si>
-  <si>
-    <t>xml2js</t>
-  </si>
-  <si>
     <t>Browserify</t>
   </si>
   <si>
@@ -172,16 +117,19 @@
   </si>
   <si>
     <t>dfahc</t>
+  </si>
+  <si>
+    <t>Decimal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -268,7 +216,7 @@
         <xdr:cNvPr id="1025" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -319,7 +267,7 @@
         <xdr:cNvPr id="2049" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000001080000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000001080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -370,7 +318,7 @@
         <xdr:cNvPr id="3073" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000010C0000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-0000010C0000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -416,7 +364,7 @@
         <xdr:cNvPr id="3" name="Imagem 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -700,32 +648,32 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="A10" sqref="A10:J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="10" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>3</v>
@@ -752,9 +700,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="4">
         <v>25.402518122853898</v>
@@ -784,13 +732,13 @@
         <v>16.2762304463945</v>
       </c>
       <c r="M2" s="2" t="str">
-        <f t="shared" ref="M2:M20" si="0">A2 &amp; " &amp; " &amp; TEXT(B2,"0.0")&amp;" &amp; "&amp;TEXT(E2,"0.0")&amp;" $\pm$ "&amp;TEXT(F2,"0.0")&amp;" &amp; "&amp;TEXT(C2,"0.0")&amp;" &amp; "&amp;TEXT(I2,"0.0")&amp;" &amp; "&amp;TEXT(G2,"0.0")&amp;" $\pm$ "&amp;TEXT(H2,"0.0")&amp;" &amp; "&amp;TEXT(D2,"0.0")&amp;" &amp; "&amp;TEXT(J2,"0.0")&amp;" \\"</f>
-        <v>browserify &amp; 25.4 &amp; 25.2 $\pm$ 0.3 &amp; 25.4 &amp; 25.4 &amp; 13.5 $\pm$ 2.9 &amp; 14.2 &amp; 16.3 \\</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+        <f>A2 &amp; " &amp; " &amp; TEXT(B2,"0.00")&amp;"\% &amp; "&amp;TEXT(C2,"0.00")&amp;"\% &amp; "&amp;TEXT(D2,"0.00")&amp;"\% &amp; "&amp;TEXT(E2,"0.00")&amp;"\% $\pm$ "&amp;TEXT(F2,"0.00")&amp;"\% &amp; "&amp;TEXT(G2,"0.00")&amp;"\% $\pm$ "&amp;TEXT(H2,"0.00")&amp;"\% &amp; "&amp;TEXT(I2,"0.00")&amp;"\% &amp; "&amp;TEXT(J2,"0.00")&amp;"\%  \\"</f>
+        <v>Browserify &amp; 25.40\% &amp; 25.40\% &amp; 14.20\% &amp; 25.25\% $\pm$ 0.32\% &amp; 13.50\% $\pm$ 2.86\% &amp; 25.40\% &amp; 16.28\%  \\</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="4">
         <v>26.001195457262401</v>
@@ -820,13 +768,13 @@
         <v>24.208009563658099</v>
       </c>
       <c r="M3" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>d3-node &amp; 26.0 &amp; 26.0 $\pm$ 0.0 &amp; 26.0 &amp; 26.0 &amp; 24.2 $\pm$ 0.0 &amp; 24.2 &amp; 24.2 \\</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+        <f t="shared" ref="M3:M20" si="0">A3 &amp; " &amp; " &amp; TEXT(B3,"0.00")&amp;"\% &amp; "&amp;TEXT(C3,"0.00")&amp;"\% &amp; "&amp;TEXT(D3,"0.00")&amp;"\% &amp; "&amp;TEXT(E3,"0.00")&amp;"\% $\pm$ "&amp;TEXT(F3,"0.00")&amp;"\% &amp; "&amp;TEXT(G3,"0.00")&amp;"\% $\pm$ "&amp;TEXT(H3,"0.00")&amp;"\% &amp; "&amp;TEXT(I3,"0.00")&amp;"\% &amp; "&amp;TEXT(J3,"0.00")&amp;"\%  \\"</f>
+        <v>D3-node &amp; 26.00\% &amp; 26.00\% &amp; 24.21\% &amp; 26.00\% $\pm$ 0.00\% &amp; 24.21\% $\pm$ 0.00\% &amp; 26.00\% &amp; 24.21\%  \\</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="B4" s="4">
         <v>14.980001269760599</v>
@@ -857,10 +805,10 @@
       </c>
       <c r="M4" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>decimal.js &amp; 15.0 &amp; 6.4 $\pm$ 2.0 &amp; 7.0 &amp; 9.2 &amp; 6.4 $\pm$ 2.0 &amp; 7.0 &amp; 9.2 \\</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+        <v>Decimal &amp; 14.98\% &amp; 6.98\% &amp; 6.98\% &amp; 6.44\% $\pm$ 2.05\% &amp; 6.44\% $\pm$ 2.05\% &amp; 9.22\% &amp; 9.22\%  \\</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -893,10 +841,10 @@
       </c>
       <c r="M5" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>esprima &amp; 3.9 &amp; 3.9 $\pm$ 0.0 &amp; 3.9 &amp; 3.9 &amp; 0.3 $\pm$ 0.1 &amp; 0.3 &amp; 0.6 \\</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+        <v>Esprima &amp; 3.88\% &amp; 3.88\% &amp; 0.33\% &amp; 3.88\% $\pm$ 0.01\% &amp; 0.35\% $\pm$ 0.11\% &amp; 3.89\% &amp; 0.64\%  \\</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -929,10 +877,10 @@
       </c>
       <c r="M6" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>exectimer &amp; 26.8 &amp; 26.4 $\pm$ 0.5 &amp; 26.8 &amp; 26.8 &amp; 22.8 $\pm$ 0.8 &amp; 23.1 &amp; 23.6 \\</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+        <v>Exectimer &amp; 26.76\% &amp; 26.76\% &amp; 23.05\% &amp; 26.37\% $\pm$ 0.50\% &amp; 22.85\% $\pm$ 0.85\% &amp; 26.76\% &amp; 23.59\%  \\</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -965,10 +913,10 @@
       </c>
       <c r="M7" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>express &amp; 15.9 &amp; 15.7 $\pm$ 0.3 &amp; 15.9 &amp; 15.9 &amp; 8.6 $\pm$ 1.3 &amp; 8.3 &amp; 11.2 \\</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+        <v>Express &amp; 15.89\% &amp; 15.86\% &amp; 8.32\% &amp; 15.70\% $\pm$ 0.30\% &amp; 8.56\% $\pm$ 1.35\% &amp; 15.89\% &amp; 11.24\%  \\</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1001,10 +949,10 @@
       </c>
       <c r="M8" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>jquery &amp; 80.1 &amp; 80.1 $\pm$ 0.0 &amp; 80.1 &amp; 80.1 &amp; 20.8 $\pm$ 3.8 &amp; 20.0 &amp; 27.8 \\</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+        <v>jQuery &amp; 80.10\% &amp; 80.05\% &amp; 20.02\% &amp; 80.05\% $\pm$ 0.03\% &amp; 20.79\% $\pm$ 3.82\% &amp; 80.13\% &amp; 27.77\%  \\</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1037,10 +985,10 @@
       </c>
       <c r="M9" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>lodash &amp; 1.6 &amp; 1.2 $\pm$ 0.3 &amp; 1.2 &amp; 1.5 &amp; 1.2 $\pm$ 0.3 &amp; 1.3 &amp; 1.6 \\</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+        <v>Lodash &amp; 1.59\% &amp; 1.22\% &amp; 1.27\% &amp; 1.20\% $\pm$ 0.26\% &amp; 1.21\% $\pm$ 0.28\% &amp; 1.48\% &amp; 1.56\%  \\</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -1073,10 +1021,10 @@
       </c>
       <c r="M10" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>mathjs &amp; 27.0 &amp; 19.1 $\pm$ 1.3 &amp; 19.0 &amp; 21.0 &amp; 19.1 $\pm$ 1.3 &amp; 19.0 &amp; 21.0 \\</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+        <v>Mathjs &amp; 27.04\% &amp; 19.04\% &amp; 19.04\% &amp; 19.07\% $\pm$ 1.27\% &amp; 19.07\% $\pm$ 1.27\% &amp; 21.00\% &amp; 21.00\%  \\</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -1109,10 +1057,10 @@
       </c>
       <c r="M11" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>minimist &amp; 2.8 &amp; 2.8 $\pm$ 0.0 &amp; 2.8 &amp; 2.8 &amp; 1.9 $\pm$ 0.1 &amp; 1.8 &amp; 2.0 \\</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+        <v>Minimist &amp; 2.78\% &amp; 2.78\% &amp; 1.84\% &amp; 2.78\% $\pm$ 0.00\% &amp; 1.85\% $\pm$ 0.08\% &amp; 2.78\% &amp; 1.96\%  \\</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -1145,10 +1093,10 @@
       </c>
       <c r="M12" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>moment &amp; 7.2 &amp; 7.1 $\pm$ 0.4 &amp; 7.2 &amp; 7.2 &amp; 1.6 $\pm$ 0.3 &amp; 1.4 &amp; 2.3 \\</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+        <v>Moment &amp; 7.23\% &amp; 7.23\% &amp; 1.43\% &amp; 7.12\% $\pm$ 0.35\% &amp; 1.55\% $\pm$ 0.34\% &amp; 7.25\% &amp; 2.32\%  \\</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -1181,10 +1129,10 @@
       </c>
       <c r="M13" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>node-semver &amp; 13.5 &amp; 13.4 $\pm$ 0.3 &amp; 13.4 &amp; 13.7 &amp; 4.4 $\pm$ 0.7 &amp; 4.1 &amp; 5.6 \\</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+        <v>Node-semver &amp; 13.46\% &amp; 13.40\% &amp; 4.12\% &amp; 13.42\% $\pm$ 0.34\% &amp; 4.35\% $\pm$ 0.65\% &amp; 13.71\% &amp; 5.61\%  \\</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -1217,10 +1165,10 @@
       </c>
       <c r="M14" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>plivo-node &amp; 15.3 &amp; 15.9 $\pm$ 0.4 &amp; 15.9 &amp; 16.4 &amp; 56.1 $\pm$ 3.0 &amp; 55.6 &amp; 61.3 \\</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+        <v>Plivo-node &amp; 15.34\% &amp; 15.90\% &amp; 55.62\% &amp; 15.92\% $\pm$ 0.38\% &amp; 56.12\% $\pm$ 2.96\% &amp; 16.38\% &amp; 61.27\%  \\</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1253,10 +1201,10 @@
       </c>
       <c r="M15" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>pug &amp; 39.4 &amp; 39.4 $\pm$ 0.0 &amp; 39.4 &amp; 39.4 &amp; 30.6 $\pm$ 2.2 &amp; 31.1 &amp; 33.9 \\</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+        <v>Pug &amp; 39.35\% &amp; 39.35\% &amp; 31.09\% &amp; 39.35\% $\pm$ 0.00\% &amp; 30.61\% $\pm$ 2.20\% &amp; 39.35\% &amp; 33.85\%  \\</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -1289,12 +1237,12 @@
       </c>
       <c r="M16" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>tleaf &amp; 65.8 &amp; 65.8 $\pm$ 0.0 &amp; 65.8 &amp; 65.8 &amp; 63.7 $\pm$ 0.8 &amp; 64.0 &amp; 64.1 \\</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+        <v>Tleaf &amp; 65.80\% &amp; 65.80\% &amp; 64.02\% &amp; 65.80\% $\pm$ 0.00\% &amp; 63.71\% $\pm$ 0.81\% &amp; 65.80\% &amp; 64.05\%  \\</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="B17" s="4">
         <v>13.2041077591005</v>
@@ -1325,10 +1273,10 @@
       </c>
       <c r="M17" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>UglifyJS2 &amp; 13.2 &amp; 12.2 $\pm$ 4.1 &amp; 13.9 &amp; 13.9 &amp; 3.1 $\pm$ 0.6 &amp; 3.1 &amp; 4.1 \\</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+        <v>UglifyJS2 &amp; 13.20\% &amp; 13.88\% &amp; 3.14\% &amp; 12.23\% $\pm$ 4.07\% &amp; 3.06\% $\pm$ 0.58\% &amp; 13.94\% &amp; 4.08\%  \\</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -1361,10 +1309,10 @@
       </c>
       <c r="M18" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>underscore &amp; 11.5 &amp; 11.5 $\pm$ 0.0 &amp; 11.5 &amp; 11.5 &amp; 4.6 $\pm$ 1.5 &amp; 4.7 &amp; 8.0 \\</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+        <v>Underscore &amp; 11.48\% &amp; 11.48\% &amp; 4.66\% &amp; 11.48\% $\pm$ 0.00\% &amp; 4.63\% $\pm$ 1.49\% &amp; 11.48\% &amp; 8.02\%  \\</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -1397,10 +1345,10 @@
       </c>
       <c r="M19" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>uuid &amp; 20.8 &amp; 21.4 $\pm$ 2.5 &amp; 22.2 &amp; 23.6 &amp; 21.5 $\pm$ 1.9 &amp; 21.6 &amp; 24.3 \\</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+        <v>UUID &amp; 20.82\% &amp; 22.15\% &amp; 21.57\% &amp; 21.43\% $\pm$ 2.49\% &amp; 21.45\% $\pm$ 1.86\% &amp; 23.63\% &amp; 24.35\%  \\</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -1408,13 +1356,13 @@
         <v>4.1199855439103796</v>
       </c>
       <c r="C20" s="4">
-        <v>-1.15046379954222</v>
+        <v>0</v>
       </c>
       <c r="D20" s="4">
         <v>9.7501819063788506</v>
       </c>
       <c r="E20" s="4">
-        <v>-2.1900975786049899</v>
+        <v>0</v>
       </c>
       <c r="F20" s="4">
         <v>4.3954368272869697</v>
@@ -1433,15 +1381,15 @@
       </c>
       <c r="M20" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>xml2js &amp; 4.1 &amp; -2.2 $\pm$ 4.4 &amp; -1.2 &amp; 2.8 &amp; 10.3 $\pm$ 5.8 &amp; 9.8 &amp; 17.6 \\</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+        <v>XML2js &amp; 4.12\% &amp; 0.00\% &amp; 9.75\% &amp; 0.00\% $\pm$ 4.40\% &amp; 10.33\% $\pm$ 5.79\% &amp; 2.79\% &amp; 17.61\%  \\</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
       <c r="A25" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>3</v>
@@ -1468,9 +1416,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13">
       <c r="A26" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="B26" s="1">
         <v>26.6</v>
@@ -1500,9 +1448,9 @@
         <v>16.3</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="B27" s="1">
         <v>29.3</v>
@@ -1532,9 +1480,9 @@
         <v>25.5</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13">
       <c r="A28" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="B28" s="1">
         <v>7.1</v>
@@ -1564,9 +1512,9 @@
         <v>6.8</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13">
       <c r="A29" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="B29" s="1">
         <v>4</v>
@@ -1596,9 +1544,9 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="B30" s="1">
         <v>22.8</v>
@@ -1628,9 +1576,9 @@
         <v>21.4</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13">
       <c r="A31" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="B31" s="1">
         <v>3.4</v>
@@ -1660,9 +1608,9 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13">
       <c r="A32" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="B32" s="1">
         <v>58.3</v>
@@ -1692,9 +1640,9 @@
         <v>25.4</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10">
       <c r="A33" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="B33" s="1">
         <v>2.7</v>
@@ -1724,9 +1672,9 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10">
       <c r="A34" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="B34" s="1">
         <v>9.8000000000000007</v>
@@ -1756,9 +1704,9 @@
         <v>17.2</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="B35" s="1">
         <v>2.8</v>
@@ -1788,9 +1736,9 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10">
       <c r="A36" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="B36" s="1">
         <v>7.1</v>
@@ -1820,9 +1768,9 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10">
       <c r="A37" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="B37" s="1">
         <v>0.2</v>
@@ -1852,9 +1800,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10">
       <c r="A38" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="B38" s="1">
         <v>33.200000000000003</v>
@@ -1884,9 +1832,9 @@
         <v>58.5</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10">
       <c r="A39" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="B39" s="1">
         <v>30.9</v>
@@ -1916,9 +1864,9 @@
         <v>26.1</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10">
       <c r="A40" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="B40" s="1">
         <v>73.8</v>
@@ -1948,9 +1896,9 @@
         <v>69.599999999999994</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10">
       <c r="A41" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="B41" s="1">
         <v>12.1</v>
@@ -1980,9 +1928,9 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10">
       <c r="A42" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="B42" s="1">
         <v>10</v>
@@ -2012,9 +1960,9 @@
         <v>6.6</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10">
       <c r="A43" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="B43" s="1">
         <v>24.3</v>
@@ -2044,9 +1992,9 @@
         <v>26.4</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10">
       <c r="A44" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="B44" s="1">
         <v>5</v>
@@ -2084,7 +2032,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -2092,7 +2040,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" scale="74" orientation="landscape" r:id="rId1"/>
@@ -2101,7 +2049,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -2111,7 +2059,7 @@
       <selection activeCell="B2" sqref="B2:T42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" scale="74" orientation="landscape" r:id="rId1"/>

</xml_diff>